<commit_message>
v5 con colores en columnas y estado
</commit_message>
<xml_diff>
--- a/dist/01_09012025.xlsx
+++ b/dist/01_09012025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\pyAlhambra\pyAlhambra\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851152BD-BD85-46B3-8473-E32538E6A3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C76548-BB88-4E10-968C-C7FFB7B995C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38292" yWindow="3744" windowWidth="29016" windowHeight="15696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="루밍" sheetId="9" r:id="rId1"/>
@@ -2436,64 +2436,64 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="29" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="18" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="30" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="31" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="27" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="28" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="13" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="24" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="25" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="26" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="23" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="29" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="25" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="26" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="30" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="31" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="23" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="29" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="29" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="18" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="27" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="28" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="13" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="24" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="25" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="26" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3306,25 +3306,25 @@
   </sheetPr>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="L22" sqref="L21:L22"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="10" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="4" max="4" width="16.6640625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:4" ht="15" thickBot="1">
       <c r="A1" s="19"/>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="31"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -3333,10 +3333,10 @@
       <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="31" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -3347,10 +3347,10 @@
       <c r="A3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="35" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -3361,10 +3361,10 @@
       <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="31" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -3375,10 +3375,10 @@
       <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="23" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="13" t="s">
@@ -3389,10 +3389,10 @@
       <c r="A6" s="16">
         <v>5</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="35" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -3403,10 +3403,10 @@
       <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="29" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="10" t="s">
@@ -3417,10 +3417,10 @@
       <c r="A8" s="12">
         <v>7</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -3431,10 +3431,10 @@
       <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="39" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -3445,10 +3445,10 @@
       <c r="A10" s="12">
         <v>9</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -3459,10 +3459,10 @@
       <c r="A11" s="16">
         <v>10</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="33" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="14" t="s">
@@ -3473,10 +3473,10 @@
       <c r="A12" s="11">
         <v>11</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="39" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -3487,10 +3487,10 @@
       <c r="A13" s="12">
         <v>12</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="35" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -3501,10 +3501,10 @@
       <c r="A14" s="11">
         <v>13</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="39" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -3515,10 +3515,10 @@
       <c r="A15" s="12">
         <v>14</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="33" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="14" t="s">
@@ -3529,10 +3529,10 @@
       <c r="A16" s="11">
         <v>15</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="39" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -3543,10 +3543,10 @@
       <c r="A17" s="18">
         <v>16</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="23" t="s">
         <v>15</v>
       </c>
       <c r="D17" s="13" t="s">
@@ -3557,10 +3557,10 @@
       <c r="A18" s="12">
         <v>17</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="27" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -3571,10 +3571,10 @@
       <c r="A19" s="11">
         <v>18</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="29" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="10" t="s">
@@ -3585,10 +3585,10 @@
       <c r="A20" s="12">
         <v>19</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="27" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -3599,10 +3599,10 @@
       <c r="A21" s="11">
         <v>20</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="29" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="10" t="s">
@@ -3613,10 +3613,10 @@
       <c r="A22" s="16">
         <v>21</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="27" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="9" t="s">
@@ -3627,10 +3627,10 @@
       <c r="A23" s="11">
         <v>22</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="29" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="10" t="s">
@@ -3641,10 +3641,10 @@
       <c r="A24" s="16">
         <v>23</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="27" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -3655,10 +3655,10 @@
       <c r="A25" s="11">
         <v>24</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="21"/>
+      <c r="C25" s="39"/>
       <c r="D25" s="7" t="s">
         <v>53</v>
       </c>
@@ -3667,10 +3667,10 @@
       <c r="A26" s="16">
         <v>25</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="23"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="5" t="s">
         <v>54</v>
       </c>
@@ -3679,10 +3679,10 @@
       <c r="A27" s="11">
         <v>26</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="21"/>
+      <c r="C27" s="39"/>
       <c r="D27" s="7" t="s">
         <v>55</v>
       </c>
@@ -3691,10 +3691,10 @@
       <c r="A28" s="16">
         <v>27</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="23"/>
+      <c r="C28" s="35"/>
       <c r="D28" s="5" t="s">
         <v>56</v>
       </c>
@@ -3703,10 +3703,10 @@
       <c r="A29" s="16">
         <v>28</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="8" t="s">
@@ -3717,16 +3717,32 @@
       <c r="A30" s="16">
         <v>29</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="35"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="8" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B30:C30"/>
@@ -3737,26 +3753,10 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -3769,14 +3769,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3b324d95-18ae-4ef0-925b-59110413f0ec" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e2096bfe-5fc0-4a56-b376-f3fe333f10a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4015,21 +4013,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3b324d95-18ae-4ef0-925b-59110413f0ec" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e2096bfe-5fc0-4a56-b376-f3fe333f10a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4522C266-632E-4F05-B2E0-760837EFC1AA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02FB0FBE-C215-4B1C-9DFA-72CA9D79BEAB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3b324d95-18ae-4ef0-925b-59110413f0ec"/>
-    <ds:schemaRef ds:uri="e2096bfe-5fc0-4a56-b376-f3fe333f10a2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4054,9 +4051,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02FB0FBE-C215-4B1C-9DFA-72CA9D79BEAB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4522C266-632E-4F05-B2E0-760837EFC1AA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3b324d95-18ae-4ef0-925b-59110413f0ec"/>
+    <ds:schemaRef ds:uri="e2096bfe-5fc0-4a56-b376-f3fe333f10a2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>